<commit_message>
added one more column
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myujung\Documents\ECAD-Test\ECAD-Test\ECAD-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9727131-01B6-40FC-8C8C-5D0E5AA1B8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC686CC-C885-4FBF-AC50-71BFD761D2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29520" yWindow="1725" windowWidth="19980" windowHeight="14820" xr2:uid="{30FE9646-959A-4F4D-B4B7-63464880FBF0}"/>
+    <workbookView xWindow="-38520" yWindow="-1545" windowWidth="38640" windowHeight="21120" xr2:uid="{30FE9646-959A-4F4D-B4B7-63464880FBF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Column1</t>
   </si>
@@ -167,24 +167,34 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="percentStacked"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$15</c:f>
@@ -236,28 +246,36 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5FF7-4EFE-8358-56DCECDEFD76}"/>
+              <c16:uniqueId val="{00000000-E8FA-43C5-919C-B383A0F96751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$15</c:f>
@@ -309,28 +327,36 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5FF7-4EFE-8358-56DCECDEFD76}"/>
+              <c16:uniqueId val="{00000001-E8FA-43C5-919C-B383A0F96751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$15</c:f>
@@ -382,28 +408,36 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5FF7-4EFE-8358-56DCECDEFD76}"/>
+              <c16:uniqueId val="{00000002-E8FA-43C5-919C-B383A0F96751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$15</c:f>
@@ -455,28 +489,36 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-5FF7-4EFE-8358-56DCECDEFD76}"/>
+              <c16:uniqueId val="{00000003-E8FA-43C5-919C-B383A0F96751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$15</c:f>
@@ -528,28 +570,36 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-5FF7-4EFE-8358-56DCECDEFD76}"/>
+              <c16:uniqueId val="{00000004-E8FA-43C5-919C-B383A0F96751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$2:$F$15</c:f>
@@ -601,30 +651,38 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-5FF7-4EFE-8358-56DCECDEFD76}"/>
+              <c16:uniqueId val="{00000005-E8FA-43C5-919C-B383A0F96751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$G$2:$G$15</c:f>
@@ -676,30 +734,38 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-5FF7-4EFE-8358-56DCECDEFD76}"/>
+              <c16:uniqueId val="{00000006-E8FA-43C5-919C-B383A0F96751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
           <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$H$2:$H$15</c:f>
@@ -751,10 +817,92 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-5FF7-4EFE-8358-56DCECDEFD76}"/>
+              <c16:uniqueId val="{00000007-E8FA-43C5-919C-B383A0F96751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-E8FA-43C5-919C-B383A0F96751}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -766,12 +914,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="189160479"/>
-        <c:axId val="189171519"/>
-      </c:lineChart>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="203808831"/>
+        <c:axId val="203802591"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="189160479"/>
+        <c:axId val="203808831"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +962,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189171519"/>
+        <c:crossAx val="203802591"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -821,7 +970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189171519"/>
+        <c:axId val="203802591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -841,7 +990,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -872,7 +1021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189160479"/>
+        <c:crossAx val="203808831"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -916,7 +1065,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1000,7 +1149,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1108,11 +1257,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1123,11 +1267,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1159,9 +1298,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1520,22 +1656,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>284797</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>399097</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F916A99A-5E46-0EE5-5EFE-051CD3388AB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58FD14B0-7FDE-83DE-77F4-A6B0557769C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1890,18 +2026,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2848F8-6F38-4853-B84C-58ACB8EA2DE5}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H15"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="10.88671875" customWidth="1"/>
+    <col min="1" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1926,8 +2062,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1952,8 +2091,11 @@
       <c r="H2">
         <v>10</v>
       </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1978,8 +2120,11 @@
       <c r="H3">
         <v>9</v>
       </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2004,8 +2149,11 @@
       <c r="H4">
         <v>8</v>
       </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2030,8 +2178,11 @@
       <c r="H5">
         <v>7</v>
       </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2056,8 +2207,11 @@
       <c r="H6">
         <v>6</v>
       </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2082,8 +2236,11 @@
       <c r="H7">
         <v>5</v>
       </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2108,8 +2265,11 @@
       <c r="H8">
         <v>4</v>
       </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2134,8 +2294,11 @@
       <c r="H9">
         <v>3</v>
       </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2160,8 +2323,11 @@
       <c r="H10">
         <v>2</v>
       </c>
+      <c r="I10">
+        <v>12</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2186,8 +2352,11 @@
       <c r="H11">
         <v>1</v>
       </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2212,8 +2381,11 @@
       <c r="H12">
         <v>0</v>
       </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2238,8 +2410,11 @@
       <c r="H13">
         <v>-1</v>
       </c>
+      <c r="I13">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2264,8 +2439,11 @@
       <c r="H14">
         <v>-2</v>
       </c>
+      <c r="I14">
+        <v>-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2288,6 +2466,9 @@
         <v>14</v>
       </c>
       <c r="H15">
+        <v>-3</v>
+      </c>
+      <c r="I15">
         <v>-3</v>
       </c>
     </row>

</xml_diff>